<commit_message>
Changes to show timestamps for timers expired
</commit_message>
<xml_diff>
--- a/resources/timerCalculation.xlsx
+++ b/resources/timerCalculation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="10935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="10935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Actual Timing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>familiarization</t>
   </si>
@@ -66,14 +67,90 @@
   </si>
   <si>
     <t>Total Duration</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Settling down</t>
+  </si>
+  <si>
+    <t>AWA Issue</t>
+  </si>
+  <si>
+    <t>Short Break</t>
+  </si>
+  <si>
+    <t>AWA Argument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbal -1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantitative -1 </t>
+  </si>
+  <si>
+    <t>Long Break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytical -1 </t>
+  </si>
+  <si>
+    <t>Verbal -2</t>
+  </si>
+  <si>
+    <t>Quantitative -2</t>
+  </si>
+  <si>
+    <t>Analytical -2</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Settling</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>Argument</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>q2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-14009]hh:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,10 +181,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,4 +911,748 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <f>C2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="G2" s="4">
+        <f>F2+H2</f>
+        <v>0.36736111111111114</v>
+      </c>
+      <c r="H2" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I2" s="4">
+        <f>G17-G2</f>
+        <v>0.13541666666666652</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="M2" s="4">
+        <f>L2+N2</f>
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="N2" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="O2" s="4">
+        <f>M17-M2</f>
+        <v>0.13980324074074058</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0.17847222222222223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3+D2</f>
+        <v>31</v>
+      </c>
+      <c r="F3" s="4">
+        <f>G2</f>
+        <v>0.36736111111111114</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G17" si="0">F3+H3</f>
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="4">
+        <f>M2</f>
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="M3" s="4">
+        <f t="shared" ref="M3:M17" si="1">L3+N3</f>
+        <v>0.37986111111111109</v>
+      </c>
+      <c r="N3" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>Q2+R2</f>
+        <v>0.53680555555555554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4+D3</f>
+        <v>32</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" ref="F4:F17" si="2">G3</f>
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H4" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J4" s="6">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4:L17" si="3">M3</f>
+        <v>0.37986111111111109</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="N4" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D17" si="4">C5+D4</f>
+        <v>62</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J5" s="6">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="3"/>
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="N5" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="H6" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J6" s="6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="3"/>
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40208333333333329</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="J7" s="6">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.40208333333333329</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40833333333333327</v>
+      </c>
+      <c r="N7" s="4">
+        <v>6.2499999999999995E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="H8" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J8" s="6">
+        <v>7</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.40833333333333327</v>
+      </c>
+      <c r="M8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40902777777777771</v>
+      </c>
+      <c r="N8" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="4"/>
+        <v>124</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="J9" s="6">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.40902777777777771</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.42591435185185178</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1.6886574074074075E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="4"/>
+        <v>134</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.44722222222222219</v>
+      </c>
+      <c r="H10" s="4">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="J10" s="6">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.42591435185185178</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.43008101851851843</v>
+      </c>
+      <c r="N10" s="4">
+        <v>4.1666666666666666E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.44722222222222219</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.45416666666666661</v>
+      </c>
+      <c r="H11" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.43008101851851843</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.45091435185185175</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.45416666666666661</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.45486111111111105</v>
+      </c>
+      <c r="H12" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J12" s="6">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.45091435185185175</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.45160879629629619</v>
+      </c>
+      <c r="N12" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.45486111111111105</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.47430555555555548</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="J13" s="6">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.45160879629629619</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.45855324074074061</v>
+      </c>
+      <c r="N13" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="4"/>
+        <v>196</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.47430555555555548</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>0.47499999999999992</v>
+      </c>
+      <c r="H14" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J14" s="6">
+        <v>13</v>
+      </c>
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.45855324074074061</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.45924768518518505</v>
+      </c>
+      <c r="N14" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="4"/>
+        <v>226</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.47499999999999992</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>0.49166666666666659</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="J15" s="6">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.45924768518518505</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.4773032407407406</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1.8055555555555557E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
+        <v>227</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="2"/>
+        <v>0.49166666666666659</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.49236111111111103</v>
+      </c>
+      <c r="H16" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J16" s="6">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.4773032407407406</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.47799768518518504</v>
+      </c>
+      <c r="N16" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="4"/>
+        <v>257</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="2"/>
+        <v>0.49236111111111103</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.50277777777777766</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="J17" s="6">
+        <v>16</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.47799768518518504</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.49883101851851835</v>
+      </c>
+      <c r="N17" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Approach 1 Commit : This is not fully functional.
</commit_message>
<xml_diff>
--- a/resources/timerCalculation.xlsx
+++ b/resources/timerCalculation.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="10935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Actual Timing" sheetId="2" r:id="rId2"/>
+    <sheet name="Work Area" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>familiarization</t>
   </si>
@@ -142,6 +143,15 @@
   </si>
   <si>
     <t>q2</t>
+  </si>
+  <si>
+    <t>Google Timer</t>
+  </si>
+  <si>
+    <t>Google Stopwatch</t>
+  </si>
+  <si>
+    <t>Countdown Timer</t>
   </si>
 </sst>
 </file>
@@ -150,7 +160,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-14009]hh:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="[$-14009]hh:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -186,7 +196,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -471,9 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -917,9 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1655,4 +1661,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.85486111111111107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>